<commit_message>
### MetaFile Generate 기능 완성.
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Core/Parser/Monster.xlsx
+++ b/Assets/Scripts/Core/Parser/Monster.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wnsrl\OneDrive\바탕 화면\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wnsrl\OneDrive\바탕 화면\Dev\IdleGameProject\Assets\Scripts\Core\Parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F00D97D-4632-41D7-9FAB-121BF31A208B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EA5D7D-87A4-4AA3-A0A6-9EDA6F419A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4230" yWindow="3075" windowWidth="19710" windowHeight="12645" xr2:uid="{96C38A8E-3BA4-4918-89A3-1A6E4E52672F}"/>
+    <workbookView xWindow="5295" yWindow="2085" windowWidth="13695" windowHeight="12645" xr2:uid="{96C38A8E-3BA4-4918-89A3-1A6E4E52672F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>fileName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -53,6 +53,18 @@
   </si>
   <si>
     <t>MON_GOBLIN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VFX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HittedVFX2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HittedVFX,HittedVFX2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -141,6 +153,16 @@
     <tableColumn id="1" xr3:uid="{D4AB0954-464D-468F-A536-29618BF9878C}" name="MaskedId" dataDxfId="0">
       <calculatedColumnFormula>IF(표1[[#This Row],[Id]]="","",_xlfn.BITOR(표1[[#This Row],[Id]],4294967296))</calculatedColumnFormula>
     </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6A1B23A3-760F-4789-9565-7F0577486AF3}" name="표3" displayName="표3" ref="D1:D101" totalsRowShown="0">
+  <autoFilter ref="D1:D101" xr:uid="{6A1B23A3-760F-4789-9565-7F0577486AF3}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{CFEADB9E-09E3-4FA0-9B5D-075D597E2670}" name="VFX"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -443,19 +465,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{330BEF0F-C7BC-4B2B-8199-B4DC333AF275}">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.875" customWidth="1"/>
-    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.25" customWidth="1"/>
+    <col min="2" max="2" width="9.625" customWidth="1"/>
+    <col min="3" max="3" width="13.125" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="17.875" customWidth="1"/>
+    <col min="6" max="6" width="14.75" customWidth="1"/>
+    <col min="7" max="7" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,8 +492,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -477,8 +507,11 @@
         <f>IF(표1[[#This Row],[Id]]="","",_xlfn.BITOR(표1[[#This Row],[Id]],4294967296))</f>
         <v>4294967297</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -489,80 +522,77 @@
         <f>IF(표1[[#This Row],[Id]]="","",_xlfn.BITOR(표1[[#This Row],[Id]],4294967296))</f>
         <v>4294967298</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C4" t="str">
-        <f>IF(표1[[#This Row],[Id]]="","",_xlfn.BITOR(표1[[#This Row],[Id]],4294967296))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C5" t="str">
         <f>IF(표1[[#This Row],[Id]]="","",_xlfn.BITOR(표1[[#This Row],[Id]],4294967296))</f>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C6" t="str">
         <f>IF(표1[[#This Row],[Id]]="","",_xlfn.BITOR(표1[[#This Row],[Id]],4294967296))</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C7" t="str">
         <f>IF(표1[[#This Row],[Id]]="","",_xlfn.BITOR(표1[[#This Row],[Id]],4294967296))</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C8" t="str">
         <f>IF(표1[[#This Row],[Id]]="","",_xlfn.BITOR(표1[[#This Row],[Id]],4294967296))</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C9" t="str">
         <f>IF(표1[[#This Row],[Id]]="","",_xlfn.BITOR(표1[[#This Row],[Id]],4294967296))</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C10" t="str">
         <f>IF(표1[[#This Row],[Id]]="","",_xlfn.BITOR(표1[[#This Row],[Id]],4294967296))</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C11" t="str">
         <f>IF(표1[[#This Row],[Id]]="","",_xlfn.BITOR(표1[[#This Row],[Id]],4294967296))</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C12" t="str">
         <f>IF(표1[[#This Row],[Id]]="","",_xlfn.BITOR(표1[[#This Row],[Id]],4294967296))</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C13" t="str">
         <f>IF(표1[[#This Row],[Id]]="","",_xlfn.BITOR(표1[[#This Row],[Id]],4294967296))</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C14" t="str">
         <f>IF(표1[[#This Row],[Id]]="","",_xlfn.BITOR(표1[[#This Row],[Id]],4294967296))</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C15" t="str">
         <f>IF(표1[[#This Row],[Id]]="","",_xlfn.BITOR(표1[[#This Row],[Id]],4294967296))</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C16" t="str">
         <f>IF(표1[[#This Row],[Id]]="","",_xlfn.BITOR(표1[[#This Row],[Id]],4294967296))</f>
         <v/>
@@ -1081,9 +1111,10 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>